<commit_message>
Fix errors and update BOM
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repo\ttk4155-PCB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE3321A1-1B7E-4857-833E-2FE3A5E4150F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1D4C24A-F88F-4EC1-BEB9-5B1711C590B6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-35850" yWindow="3480" windowWidth="14400" windowHeight="7365" xr2:uid="{8A13EB2E-6BCF-40F7-89A4-0CF95165FE5D}"/>
+    <workbookView xWindow="-4700" yWindow="2240" windowWidth="9600" windowHeight="4910" xr2:uid="{8A13EB2E-6BCF-40F7-89A4-0CF95165FE5D}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="90">
   <si>
     <t>Component</t>
   </si>
@@ -295,6 +295,12 @@
   </si>
   <si>
     <t>AE10921-ND</t>
+  </si>
+  <si>
+    <t>I handleliste</t>
+  </si>
+  <si>
+    <t>j</t>
   </si>
 </sst>
 </file>
@@ -646,10 +652,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7054ED01-8302-4340-8F6B-B311F1132602}">
-  <dimension ref="A1:D32"/>
+  <dimension ref="A1:F32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -659,7 +665,7 @@
     <col min="4" max="4" width="24.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -672,8 +678,11 @@
       <c r="D1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="F1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -686,8 +695,11 @@
       <c r="D2" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="F2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -700,8 +712,11 @@
       <c r="D3" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="F3" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -714,8 +729,11 @@
       <c r="D4" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="F4" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -728,8 +746,11 @@
       <c r="D5" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="F5" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>86</v>
       </c>
@@ -742,8 +763,11 @@
       <c r="D6" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="F6" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>85</v>
       </c>
@@ -756,8 +780,11 @@
       <c r="D7" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="F7" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -770,8 +797,11 @@
       <c r="D8" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="F8" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -784,8 +814,11 @@
       <c r="D9" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="F9" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>60</v>
       </c>
@@ -798,8 +831,11 @@
       <c r="D10" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="F10" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>19</v>
       </c>
@@ -812,8 +848,11 @@
       <c r="D11" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="F11" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>21</v>
       </c>
@@ -826,8 +865,11 @@
       <c r="D12" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="F12" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>23</v>
       </c>
@@ -840,8 +882,11 @@
       <c r="D13" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="F13" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>25</v>
       </c>
@@ -854,8 +899,11 @@
       <c r="D14" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="F14" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>27</v>
       </c>
@@ -868,8 +916,11 @@
       <c r="D15" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="F15" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>29</v>
       </c>
@@ -882,8 +933,11 @@
       <c r="D16" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="F16" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>31</v>
       </c>
@@ -896,8 +950,11 @@
       <c r="D17" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="F17" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>34</v>
       </c>
@@ -910,8 +967,11 @@
       <c r="D18" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="F18" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>36</v>
       </c>
@@ -924,8 +984,11 @@
       <c r="D19" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="F19" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>38</v>
       </c>
@@ -938,8 +1001,11 @@
       <c r="D20" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="F20" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>40</v>
       </c>
@@ -952,8 +1018,11 @@
       <c r="D21" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="F21" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>42</v>
       </c>
@@ -966,8 +1035,11 @@
       <c r="D22" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="F22" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>44</v>
       </c>
@@ -980,8 +1052,11 @@
       <c r="D23" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="F23" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>46</v>
       </c>
@@ -994,8 +1069,11 @@
       <c r="D24" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="F24" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>48</v>
       </c>
@@ -1008,8 +1086,11 @@
       <c r="D25" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="F25" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>50</v>
       </c>
@@ -1022,8 +1103,11 @@
       <c r="D26" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="F26" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>53</v>
       </c>
@@ -1036,8 +1120,11 @@
       <c r="D27" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="F27" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>76</v>
       </c>
@@ -1050,8 +1137,11 @@
       <c r="D28" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="F28" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>55</v>
       </c>
@@ -1064,8 +1154,11 @@
       <c r="D29" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="F29" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>81</v>
       </c>
@@ -1075,8 +1168,11 @@
       <c r="D31" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="F31" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>83</v>
       </c>
@@ -1085,6 +1181,9 @@
       </c>
       <c r="D32" t="s">
         <v>84</v>
+      </c>
+      <c r="F32" t="s">
+        <v>89</v>
       </c>
     </row>
   </sheetData>

</xml_diff>